<commit_message>
updated 1968 West Virginia-Virgin Islands
</commit_message>
<xml_diff>
--- a/Output/1968/West Virginia-Virign Islands/West Virginia-Virgin Islands.xlsx
+++ b/Output/1968/West Virginia-Virign Islands/West Virginia-Virgin Islands.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunhao/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/SanDisk/Cable/Output/1968/West Virginia-Virign Islands/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,6 +17,11 @@
     <sheet name="Wyoming" sheetId="4" r:id="rId3"/>
     <sheet name="Guam, Virgin Islands" sheetId="5" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'West Virginia'!$D$1:$J$156</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Wisconsin!$D$1:$J$213</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Wyoming!$D$1:$J$37</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2521" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2516" uniqueCount="375">
   <si>
     <t>Name</t>
   </si>
@@ -791,9 +796,6 @@
     <t>MENOMONIE</t>
   </si>
   <si>
-    <t>N A</t>
-  </si>
-  <si>
     <t>Menomonee Falls</t>
   </si>
   <si>
@@ -1083,9 +1085,6 @@
   </si>
   <si>
     <t>PINE BLUFFS</t>
-  </si>
-  <si>
-    <t>uly 1, 1957</t>
   </si>
   <si>
     <t>POWELL</t>
@@ -1156,10 +1155,6 @@
   </si>
   <si>
     <t>East Bank</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dec. 1, 1952</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1871,8 +1866,8 @@
       <c r="D11">
         <v>728</v>
       </c>
-      <c r="E11" t="s">
-        <v>375</v>
+      <c r="E11" s="3">
+        <v>19329</v>
       </c>
       <c r="F11">
         <v>155</v>
@@ -1883,8 +1878,8 @@
       <c r="H11">
         <v>200</v>
       </c>
-      <c r="I11" t="s">
-        <v>13</v>
+      <c r="I11">
+        <v>5</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -2281,7 +2276,7 @@
     </row>
     <row r="25" spans="1:12">
       <c r="A25" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -2302,13 +2297,13 @@
         <v>13</v>
       </c>
       <c r="I25" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J25" t="s">
         <v>13</v>
       </c>
       <c r="K25" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="L25" t="s">
         <v>111</v>
@@ -3199,7 +3194,7 @@
     </row>
     <row r="55" spans="1:12">
       <c r="A55" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -5029,7 +5024,7 @@
     </row>
     <row r="115" spans="1:11">
       <c r="A115" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B115">
         <v>0</v>
@@ -5099,7 +5094,7 @@
         <v>1952</v>
       </c>
       <c r="F117" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="G117" t="s">
         <v>33</v>
@@ -5516,7 +5511,7 @@
         <v>1</v>
       </c>
       <c r="C138" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="139" spans="1:3">
@@ -8554,8 +8549,8 @@
       <c r="H83" s="1">
         <v>4200</v>
       </c>
-      <c r="I83" t="s">
-        <v>13</v>
+      <c r="I83">
+        <v>12</v>
       </c>
       <c r="J83">
         <v>0</v>
@@ -8855,7 +8850,7 @@
         <v>1050</v>
       </c>
       <c r="G92" t="s">
-        <v>254</v>
+        <v>373</v>
       </c>
       <c r="H92" s="1">
         <v>1500</v>
@@ -8863,13 +8858,13 @@
       <c r="I92">
         <v>12</v>
       </c>
-      <c r="J92" t="s">
-        <v>13</v>
+      <c r="J92">
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:12">
       <c r="A93" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B93">
         <v>0</v>
@@ -8904,7 +8899,7 @@
     </row>
     <row r="94" spans="1:12">
       <c r="A94" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B94">
         <v>0</v>
@@ -8939,7 +8934,7 @@
     </row>
     <row r="95" spans="1:12">
       <c r="A95" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B95">
         <v>0</v>
@@ -8974,7 +8969,7 @@
     </row>
     <row r="96" spans="1:12">
       <c r="A96" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B96">
         <v>0</v>
@@ -9003,7 +8998,7 @@
     </row>
     <row r="97" spans="1:12">
       <c r="A97" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B97">
         <v>0</v>
@@ -9038,7 +9033,7 @@
     </row>
     <row r="98" spans="1:12">
       <c r="A98" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B98">
         <v>0</v>
@@ -9073,7 +9068,7 @@
     </row>
     <row r="99" spans="1:12">
       <c r="A99" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B99">
         <v>0</v>
@@ -9108,7 +9103,7 @@
     </row>
     <row r="100" spans="1:12">
       <c r="A100" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B100">
         <v>0</v>
@@ -9143,7 +9138,7 @@
     </row>
     <row r="101" spans="1:12">
       <c r="A101" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B101">
         <v>0</v>
@@ -9178,7 +9173,7 @@
     </row>
     <row r="102" spans="1:12">
       <c r="A102" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B102">
         <v>0</v>
@@ -9213,7 +9208,7 @@
     </row>
     <row r="103" spans="1:12">
       <c r="A103" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B103">
         <v>0</v>
@@ -9248,7 +9243,7 @@
     </row>
     <row r="104" spans="1:12">
       <c r="A104" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B104">
         <v>0</v>
@@ -9283,7 +9278,7 @@
     </row>
     <row r="105" spans="1:12">
       <c r="A105" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B105">
         <v>0</v>
@@ -9318,7 +9313,7 @@
     </row>
     <row r="106" spans="1:12">
       <c r="A106" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B106">
         <v>0</v>
@@ -9353,7 +9348,7 @@
     </row>
     <row r="107" spans="1:12">
       <c r="A107" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B107">
         <v>0</v>
@@ -9388,7 +9383,7 @@
     </row>
     <row r="108" spans="1:12">
       <c r="A108" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B108">
         <v>0</v>
@@ -9423,7 +9418,7 @@
     </row>
     <row r="109" spans="1:12">
       <c r="A109" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B109">
         <v>0</v>
@@ -9458,7 +9453,7 @@
     </row>
     <row r="110" spans="1:12">
       <c r="A110" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B110">
         <v>0</v>
@@ -9493,7 +9488,7 @@
     </row>
     <row r="111" spans="1:12">
       <c r="A111" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B111">
         <v>0</v>
@@ -9528,7 +9523,7 @@
     </row>
     <row r="112" spans="1:12">
       <c r="A112" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B112">
         <v>0</v>
@@ -9563,7 +9558,7 @@
     </row>
     <row r="113" spans="1:12">
       <c r="A113" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B113">
         <v>0</v>
@@ -9598,7 +9593,7 @@
     </row>
     <row r="114" spans="1:12">
       <c r="A114" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B114">
         <v>0</v>
@@ -9633,7 +9628,7 @@
     </row>
     <row r="115" spans="1:12">
       <c r="A115" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B115">
         <v>0</v>
@@ -9668,7 +9663,7 @@
     </row>
     <row r="116" spans="1:12">
       <c r="A116" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B116">
         <v>0</v>
@@ -9703,7 +9698,7 @@
     </row>
     <row r="117" spans="1:12">
       <c r="A117" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B117">
         <v>0</v>
@@ -9732,7 +9727,7 @@
     </row>
     <row r="118" spans="1:12">
       <c r="A118" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B118">
         <v>0</v>
@@ -9767,7 +9762,7 @@
     </row>
     <row r="119" spans="1:12">
       <c r="A119" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B119">
         <v>0</v>
@@ -9802,7 +9797,7 @@
     </row>
     <row r="120" spans="1:12">
       <c r="A120" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B120">
         <v>0</v>
@@ -9837,7 +9832,7 @@
     </row>
     <row r="121" spans="1:12">
       <c r="A121" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B121">
         <v>0</v>
@@ -9872,7 +9867,7 @@
     </row>
     <row r="122" spans="1:12">
       <c r="A122" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B122">
         <v>0</v>
@@ -9907,7 +9902,7 @@
     </row>
     <row r="123" spans="1:12">
       <c r="A123" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B123">
         <v>0</v>
@@ -9942,7 +9937,7 @@
     </row>
     <row r="124" spans="1:12">
       <c r="A124" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B124">
         <v>0</v>
@@ -9977,7 +9972,7 @@
     </row>
     <row r="125" spans="1:12">
       <c r="A125" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B125">
         <v>0</v>
@@ -10012,7 +10007,7 @@
     </row>
     <row r="126" spans="1:12">
       <c r="A126" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B126">
         <v>0</v>
@@ -10047,7 +10042,7 @@
     </row>
     <row r="127" spans="1:12">
       <c r="A127" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B127">
         <v>0</v>
@@ -10082,7 +10077,7 @@
     </row>
     <row r="128" spans="1:12">
       <c r="A128" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B128">
         <v>0</v>
@@ -10117,7 +10112,7 @@
     </row>
     <row r="129" spans="1:12">
       <c r="A129" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B129">
         <v>0</v>
@@ -10152,7 +10147,7 @@
     </row>
     <row r="130" spans="1:12">
       <c r="A130" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B130">
         <v>0</v>
@@ -10181,7 +10176,7 @@
     </row>
     <row r="131" spans="1:12">
       <c r="A131" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B131">
         <v>0</v>
@@ -10213,7 +10208,7 @@
     </row>
     <row r="132" spans="1:12">
       <c r="A132" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B132">
         <v>0</v>
@@ -10242,7 +10237,7 @@
     </row>
     <row r="133" spans="1:12">
       <c r="A133" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B133">
         <v>0</v>
@@ -10277,7 +10272,7 @@
     </row>
     <row r="134" spans="1:12">
       <c r="A134" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B134">
         <v>0</v>
@@ -10312,7 +10307,7 @@
     </row>
     <row r="135" spans="1:12">
       <c r="A135" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B135">
         <v>0</v>
@@ -10347,7 +10342,7 @@
     </row>
     <row r="136" spans="1:12">
       <c r="A136" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B136">
         <v>0</v>
@@ -10382,7 +10377,7 @@
     </row>
     <row r="137" spans="1:12">
       <c r="A137" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B137">
         <v>0</v>
@@ -10417,7 +10412,7 @@
     </row>
     <row r="138" spans="1:12">
       <c r="A138" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B138">
         <v>0</v>
@@ -10452,7 +10447,7 @@
     </row>
     <row r="139" spans="1:12">
       <c r="A139" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B139">
         <v>0</v>
@@ -10487,7 +10482,7 @@
     </row>
     <row r="140" spans="1:12">
       <c r="A140" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B140">
         <v>0</v>
@@ -10522,7 +10517,7 @@
     </row>
     <row r="141" spans="1:12">
       <c r="A141" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B141">
         <v>0</v>
@@ -10557,7 +10552,7 @@
     </row>
     <row r="142" spans="1:12">
       <c r="A142" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B142">
         <v>0</v>
@@ -10592,7 +10587,7 @@
     </row>
     <row r="143" spans="1:12">
       <c r="A143" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B143">
         <v>0</v>
@@ -10621,7 +10616,7 @@
     </row>
     <row r="144" spans="1:12">
       <c r="A144" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B144">
         <v>0</v>
@@ -10656,7 +10651,7 @@
     </row>
     <row r="145" spans="1:12">
       <c r="A145" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B145">
         <v>0</v>
@@ -10691,7 +10686,7 @@
     </row>
     <row r="146" spans="1:12">
       <c r="A146" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B146">
         <v>0</v>
@@ -10726,7 +10721,7 @@
     </row>
     <row r="147" spans="1:12">
       <c r="A147" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B147">
         <v>0</v>
@@ -10755,7 +10750,7 @@
     </row>
     <row r="148" spans="1:12">
       <c r="A148" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B148">
         <v>0</v>
@@ -10784,7 +10779,7 @@
     </row>
     <row r="149" spans="1:12">
       <c r="A149" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B149">
         <v>0</v>
@@ -10813,7 +10808,7 @@
     </row>
     <row r="150" spans="1:12">
       <c r="A150" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B150">
         <v>0</v>
@@ -10848,7 +10843,7 @@
     </row>
     <row r="151" spans="1:12">
       <c r="A151" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B151">
         <v>0</v>
@@ -10883,7 +10878,7 @@
     </row>
     <row r="152" spans="1:12">
       <c r="A152" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B152">
         <v>0</v>
@@ -10915,7 +10910,7 @@
     </row>
     <row r="153" spans="1:12">
       <c r="A153" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B153">
         <v>0</v>
@@ -10950,7 +10945,7 @@
     </row>
     <row r="154" spans="1:12">
       <c r="A154" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B154">
         <v>0</v>
@@ -10985,7 +10980,7 @@
     </row>
     <row r="155" spans="1:12">
       <c r="A155" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B155">
         <v>0</v>
@@ -11020,7 +11015,7 @@
     </row>
     <row r="156" spans="1:12">
       <c r="A156" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B156">
         <v>0</v>
@@ -11055,7 +11050,7 @@
     </row>
     <row r="157" spans="1:12">
       <c r="A157" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B157">
         <v>0</v>
@@ -11084,7 +11079,7 @@
     </row>
     <row r="158" spans="1:12">
       <c r="A158" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B158">
         <v>0</v>
@@ -11119,7 +11114,7 @@
     </row>
     <row r="159" spans="1:12">
       <c r="A159" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B159">
         <v>0</v>
@@ -11154,7 +11149,7 @@
     </row>
     <row r="160" spans="1:12">
       <c r="A160" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B160">
         <v>0</v>
@@ -11183,7 +11178,7 @@
     </row>
     <row r="161" spans="1:12">
       <c r="A161" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B161">
         <v>0</v>
@@ -11215,7 +11210,7 @@
     </row>
     <row r="162" spans="1:12">
       <c r="A162" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B162">
         <v>0</v>
@@ -11244,7 +11239,7 @@
     </row>
     <row r="163" spans="1:12">
       <c r="A163" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B163">
         <v>0</v>
@@ -11273,7 +11268,7 @@
     </row>
     <row r="164" spans="1:12">
       <c r="A164" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B164">
         <v>0</v>
@@ -11308,7 +11303,7 @@
     </row>
     <row r="165" spans="1:12">
       <c r="A165" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B165">
         <v>0</v>
@@ -11337,7 +11332,7 @@
     </row>
     <row r="166" spans="1:12">
       <c r="A166" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B166">
         <v>0</v>
@@ -11372,7 +11367,7 @@
     </row>
     <row r="167" spans="1:12">
       <c r="A167" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B167">
         <v>0</v>
@@ -11407,7 +11402,7 @@
     </row>
     <row r="168" spans="1:12">
       <c r="A168" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B168">
         <v>0</v>
@@ -11442,7 +11437,7 @@
     </row>
     <row r="169" spans="1:12">
       <c r="A169" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B169">
         <v>0</v>
@@ -11477,7 +11472,7 @@
     </row>
     <row r="170" spans="1:12">
       <c r="A170" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B170">
         <v>0</v>
@@ -11512,7 +11507,7 @@
     </row>
     <row r="171" spans="1:12">
       <c r="A171" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B171">
         <v>0</v>
@@ -11547,7 +11542,7 @@
     </row>
     <row r="172" spans="1:12">
       <c r="A172" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B172">
         <v>0</v>
@@ -11582,7 +11577,7 @@
     </row>
     <row r="173" spans="1:12">
       <c r="A173" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B173">
         <v>0</v>
@@ -11617,7 +11612,7 @@
     </row>
     <row r="174" spans="1:12">
       <c r="A174" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B174">
         <v>0</v>
@@ -11652,7 +11647,7 @@
     </row>
     <row r="175" spans="1:12">
       <c r="A175" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B175">
         <v>0</v>
@@ -11687,7 +11682,7 @@
     </row>
     <row r="176" spans="1:12">
       <c r="A176" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B176">
         <v>0</v>
@@ -11722,7 +11717,7 @@
     </row>
     <row r="177" spans="1:12">
       <c r="A177" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B177">
         <v>0</v>
@@ -11754,7 +11749,7 @@
     </row>
     <row r="178" spans="1:12">
       <c r="A178" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B178">
         <v>0</v>
@@ -11789,7 +11784,7 @@
     </row>
     <row r="179" spans="1:12">
       <c r="A179" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B179">
         <v>0</v>
@@ -11824,7 +11819,7 @@
     </row>
     <row r="180" spans="1:12">
       <c r="A180" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B180">
         <v>0</v>
@@ -11859,7 +11854,7 @@
     </row>
     <row r="181" spans="1:12">
       <c r="A181" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B181">
         <v>0</v>
@@ -11888,7 +11883,7 @@
     </row>
     <row r="182" spans="1:12">
       <c r="A182" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B182">
         <v>0</v>
@@ -11923,7 +11918,7 @@
     </row>
     <row r="183" spans="1:12">
       <c r="A183" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B183">
         <v>0</v>
@@ -11958,7 +11953,7 @@
     </row>
     <row r="184" spans="1:12">
       <c r="A184" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B184">
         <v>0</v>
@@ -11990,7 +11985,7 @@
     </row>
     <row r="185" spans="1:12">
       <c r="A185" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B185">
         <v>0</v>
@@ -12025,7 +12020,7 @@
     </row>
     <row r="186" spans="1:12">
       <c r="A186" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B186">
         <v>0</v>
@@ -12060,7 +12055,7 @@
     </row>
     <row r="187" spans="1:12">
       <c r="A187" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B187">
         <v>0</v>
@@ -12095,7 +12090,7 @@
     </row>
     <row r="188" spans="1:12">
       <c r="A188" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B188">
         <v>0</v>
@@ -12124,7 +12119,7 @@
     </row>
     <row r="189" spans="1:12">
       <c r="A189" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B189">
         <v>0</v>
@@ -12159,7 +12154,7 @@
     </row>
     <row r="190" spans="1:12">
       <c r="A190" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B190">
         <v>0</v>
@@ -12194,7 +12189,7 @@
     </row>
     <row r="191" spans="1:12">
       <c r="A191" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B191">
         <v>0</v>
@@ -12229,7 +12224,7 @@
     </row>
     <row r="192" spans="1:12">
       <c r="A192" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B192">
         <v>0</v>
@@ -12264,7 +12259,7 @@
     </row>
     <row r="193" spans="1:12">
       <c r="A193" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B193">
         <v>0</v>
@@ -12299,7 +12294,7 @@
     </row>
     <row r="194" spans="1:12">
       <c r="A194" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B194">
         <v>0</v>
@@ -12334,7 +12329,7 @@
     </row>
     <row r="195" spans="1:12">
       <c r="A195" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B195">
         <v>0</v>
@@ -12369,7 +12364,7 @@
     </row>
     <row r="196" spans="1:12">
       <c r="A196" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B196">
         <v>0</v>
@@ -12404,7 +12399,7 @@
     </row>
     <row r="197" spans="1:12">
       <c r="A197" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B197">
         <v>0</v>
@@ -12439,7 +12434,7 @@
     </row>
     <row r="198" spans="1:12">
       <c r="A198" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B198">
         <v>0</v>
@@ -12468,7 +12463,7 @@
     </row>
     <row r="199" spans="1:12">
       <c r="A199" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B199">
         <v>0</v>
@@ -12503,7 +12498,7 @@
     </row>
     <row r="200" spans="1:12">
       <c r="A200" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B200">
         <v>0</v>
@@ -12645,35 +12640,35 @@
     </row>
     <row r="211" spans="1:3">
       <c r="A211" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B211">
         <v>1</v>
       </c>
       <c r="C211" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="212" spans="1:3">
       <c r="A212" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B212">
         <v>1</v>
       </c>
       <c r="C212" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="213" spans="1:3">
       <c r="A213" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B213">
         <v>1</v>
       </c>
       <c r="C213" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
   </sheetData>
@@ -12689,9 +12684,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E3964FA-EB32-EE49-AEDA-FFBB42A083C4}">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:L1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -12738,7 +12731,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -12767,7 +12760,7 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -12796,7 +12789,7 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -12825,7 +12818,7 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -12857,7 +12850,7 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -12886,7 +12879,7 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -12918,7 +12911,7 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -12953,7 +12946,7 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -12982,7 +12975,7 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -13011,7 +13004,7 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -13040,7 +13033,7 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -13069,7 +13062,7 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -13098,7 +13091,7 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -13127,7 +13120,7 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -13162,7 +13155,7 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -13197,42 +13190,42 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17" t="s">
+        <v>343</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" t="s">
+        <v>13</v>
+      </c>
+      <c r="J17" t="s">
+        <v>13</v>
+      </c>
+      <c r="K17" t="s">
+        <v>14</v>
+      </c>
+      <c r="L17" t="s">
         <v>344</v>
-      </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="D17" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" t="s">
-        <v>13</v>
-      </c>
-      <c r="G17" t="s">
-        <v>13</v>
-      </c>
-      <c r="H17" t="s">
-        <v>13</v>
-      </c>
-      <c r="I17" t="s">
-        <v>13</v>
-      </c>
-      <c r="J17" t="s">
-        <v>13</v>
-      </c>
-      <c r="K17" t="s">
-        <v>14</v>
-      </c>
-      <c r="L17" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -13261,7 +13254,7 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -13296,7 +13289,7 @@
     </row>
     <row r="20" spans="1:12">
       <c r="A20" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -13331,7 +13324,7 @@
     </row>
     <row r="21" spans="1:12">
       <c r="A21" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -13339,8 +13332,8 @@
       <c r="D21" s="1">
         <v>1121</v>
       </c>
-      <c r="E21" t="s">
-        <v>352</v>
+      <c r="E21" s="3">
+        <v>21002</v>
       </c>
       <c r="F21">
         <v>238</v>
@@ -13360,7 +13353,7 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -13389,7 +13382,7 @@
     </row>
     <row r="23" spans="1:12">
       <c r="A23" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -13418,7 +13411,7 @@
     </row>
     <row r="24" spans="1:12">
       <c r="A24" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -13447,7 +13440,7 @@
     </row>
     <row r="25" spans="1:12">
       <c r="A25" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -13476,7 +13469,7 @@
     </row>
     <row r="26" spans="1:12">
       <c r="A26" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -13505,7 +13498,7 @@
     </row>
     <row r="27" spans="1:12">
       <c r="A27" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -13534,7 +13527,7 @@
     </row>
     <row r="28" spans="1:12">
       <c r="A28" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -13563,7 +13556,7 @@
     </row>
     <row r="29" spans="1:12">
       <c r="A29" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -13592,7 +13585,7 @@
     </row>
     <row r="30" spans="1:12">
       <c r="A30" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -13621,7 +13614,7 @@
     </row>
     <row r="31" spans="1:12">
       <c r="A31" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -13650,68 +13643,68 @@
     </row>
     <row r="32" spans="1:12">
       <c r="A32" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B37">
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -13774,7 +13767,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -13789,7 +13782,7 @@
         <v>25</v>
       </c>
       <c r="G2" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="H2" t="s">
         <v>13</v>
@@ -13803,7 +13796,7 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B3">
         <v>0</v>

</xml_diff>